<commit_message>
Changed EntryHandler class into functions. Employee selection page now inline with project standard. Working on proper row population.
</commit_message>
<xml_diff>
--- a/test/German_SAPX_Extract_Augmented.xlsx
+++ b/test/German_SAPX_Extract_Augmented.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SW Development\Python\ProjectHoursBudgeter\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C56E80-D2ED-4409-9EA5-F67D044507E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F54BFFA-3630-4E4F-ABFD-30D64B159D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="2385" windowWidth="16410" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1425" yWindow="2730" windowWidth="16410" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -490,6 +490,7 @@
     <col min="2" max="2" width="45.5703125" customWidth="1"/>
     <col min="3" max="3" width="32.5703125" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>